<commit_message>
create json format to upload
</commit_message>
<xml_diff>
--- a/botc_character_list.xlsx
+++ b/botc_character_list.xlsx
@@ -473,7 +473,7 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Butler</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -483,10 +483,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>If you died today or tonight, the Demon may choose 2 players (not another Demon) to swap characters.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Each night, choose a player (not yourself): tomorrow, you may only vote if they are voting too.</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -494,7 +496,7 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Damsel</t>
+          <t>Drunk</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -504,7 +506,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>All Minions know a Damsel is in play. If a Minion publicly guesses you (once), your team loses.</t>
+          <t>You do not know you are the Drunk. You think you are a Townsfolk character, but you are not.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -515,7 +517,7 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tinker</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -525,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>You might die at any time.</t>
+          <t>If you died today or tonight, the Demon may choose 2 players (not another Demon) to swap characters.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -536,7 +538,7 @@
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>Drunk</t>
+          <t>Damsel</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -546,7 +548,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>You do not know you are the Drunk. You think you are a Townsfolk character, but you are not.</t>
+          <t>All Minions know a Damsel is in play. If a Minion publicly guesses you (once), your team loses.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -557,7 +559,7 @@
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>Heretic</t>
+          <t>Golem</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -567,18 +569,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Whoever wins, loses &amp; whoever loses, wins, even if you are dead.</t>
+          <t>You may only nominate once per game. When you do, if the nominee is not the Demon, they die.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>Puzzlemaster</t>
+          <t>Hatter</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -588,7 +592,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1 player is drunk, even if you die. If you guess (once) who it is, learn the Demon player, but guess wrong &amp; get false info.</t>
+          <t>If you died today or tonight, the Minion &amp; Demon players may choose new Minion &amp; Demon characters to be.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -599,7 +603,7 @@
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hatter</t>
+          <t>Saint</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -609,7 +613,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>If you died today or tonight, the Minion &amp; Demon players may choose new Minion &amp; Demon characters to be.</t>
+          <t>If you die by execution, your team loses.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -620,7 +624,7 @@
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>Goon</t>
+          <t>Klutz</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -630,12 +634,10 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Each night, the 1st player to choose you with their ability is drunk until dusk. You become their alignment.</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
+          <t>When you learn that you died, publicly choose 1 alive player: if they are evil, your team loses.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
@@ -643,7 +645,7 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Zealot</t>
+          <t>Goon</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -653,10 +655,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>If there are 5 or more players alive, you must vote for every nomination.</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>Each night, the 1st player to choose you with their ability is drunk until dusk. You become their alignment.</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
@@ -664,17 +668,17 @@
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Leviathan</t>
+          <t>Boffin</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>If more than 1 good player is executed, evil wins. All players know you are in play. After day 5, evil wins.</t>
+          <t>The Demon (even if drunk or poisoned) has a not-in-play good character's ability. You both know which.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -685,7 +689,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Butler</t>
+          <t>Heretic</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -695,12 +699,10 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Each night, choose a player (not yourself): tomorrow, you may only vote if they are voting too.</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
+          <t>Whoever wins, loses &amp; whoever loses, wins, even if you are dead.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -708,45 +710,41 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>Golem</t>
+          <t>Baron</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>You may only nominate once per game. When you do, if the nominee is not the Demon, they die.</t>
+          <t>There are extra Outsiders in play. [+2 Outsiders]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="n">
-        <v>1</v>
-      </c>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>Al-Hadikhia</t>
+          <t>Mutant</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Each night*, you may choose 3 players (all players learn who): each silently chooses to live or die, but if all live, all die.</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
+          <t xml:space="preserve">If you are </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
@@ -754,7 +752,7 @@
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>Moonchild</t>
+          <t>Puzzlemaster</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -764,7 +762,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>When you learn that you died, publicly choose 1 alive player. Tonight, if it was a good player, they die.</t>
+          <t>1 player is drunk, even if you die. If you guess (once) who it is, learn the Demon player, but guess wrong &amp; get false info.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -775,22 +773,20 @@
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>Imp</t>
+          <t>Snitch</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. If you kill yourself this way, a Minion becomes the Imp.</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
+          <t>Each Minion gets 3 bluffs.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
@@ -798,7 +794,7 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>Snitch</t>
+          <t>Recluse</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -808,7 +804,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Each Minion gets 3 bluffs.</t>
+          <t>You might register as evil &amp; as a Minion or Demon, even if dead.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -819,7 +815,7 @@
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sweetheart</t>
+          <t>Tinker</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -829,7 +825,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>When you die, 1 player is drunk from now on.</t>
+          <t>You might die at any time.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -840,7 +836,7 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>Klutz</t>
+          <t>Ogre</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -850,7 +846,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>When you learn that you died, publicly choose 1 alive player: if they are evil, your team loses.</t>
+          <t>No quoted ability text found</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -861,7 +857,7 @@
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>Saint</t>
+          <t>Lunatic</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -871,7 +867,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>If you die by execution, your team loses.</t>
+          <t>You think you are a Demon, but you are not. The Demon knows who you are &amp; who you choose at night.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -882,53 +878,53 @@
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lleech</t>
+          <t>Cerenovus</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. You start by choosing a player: they are poisoned. You die if &amp; only if they are dead.</t>
+          <t xml:space="preserve">Each night, choose a player &amp; a good character: they are </t>
         </is>
       </c>
       <c r="E22" t="n">
         <v>1</v>
       </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>Recluse</t>
+          <t>Assassin</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>You might register as evil &amp; as a Minion or Demon, even if dead.</t>
+          <t>Once per game, at night*, choose a player: they die, even if for some reason they could not.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mutant</t>
+          <t>Sweetheart</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -938,7 +934,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">If you are </t>
+          <t>When you die, 1 player is drunk from now on.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -949,17 +945,17 @@
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fang Gu</t>
+          <t>Fearmonger</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. The 1st Outsider this kills becomes an evil Fang Gu &amp; you die instead. [+1 Outsider]</t>
+          <t>Each night, choose a player: if you nominate &amp; execute them, their team loses. All players know if you choose a new player.</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -972,22 +968,20 @@
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>Ojo</t>
+          <t>Zealot</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Each night*, choose a character: they die. If they are not in play, the Storyteller chooses who dies.</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>1</v>
-      </c>
+          <t>If there are 5 or more players alive, you must vote for every nomination.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
@@ -995,22 +989,20 @@
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>Po</t>
+          <t>Boomdandy</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Each night*, you may choose a player: they die. If your last choice was no-one, choose 3 players tonight.</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>1</v>
-      </c>
+          <t>If you are executed, all but 3 players die. After a 10 to 1 countdown, the player with the most players pointing at them, dies.</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
@@ -1018,22 +1010,20 @@
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>Pukka</t>
+          <t>Moonchild</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Each night, choose a player: they are poisoned. The previously poisoned player dies then becomes healthy.</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>1</v>
-      </c>
+          <t>When you learn that you died, publicly choose 1 alive player. Tonight, if it was a good player, they die.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
@@ -1041,17 +1031,17 @@
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>Riot</t>
+          <t>Politician</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>On day 3, Minions become Riot &amp; nominees die but nominate an alive player immediately. This must happen.</t>
+          <t>If you were the player most responsible for your team losing, you change alignment &amp; win, even if dead.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1062,22 +1052,20 @@
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>Shabaloth</t>
+          <t>Plague Doctor</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Each night*, choose 2 players: they die. A dead player you chose last night might be regurgitated.</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>1</v>
-      </c>
+          <t>When you die, the Storyteller gains a Minion ability.</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
@@ -1085,111 +1073,107 @@
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>Vigormortis</t>
+          <t>Godfather</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. Minions you kill keep their ability &amp; poison 1 Townsfolk neighbor. [-1 Outsider]</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" t="inlineStr"/>
+          <t>You start knowing which Outsiders are in play. If 1 died today, choose a player tonight: they die. [-1 or +1 Outsider]</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>Vortox</t>
+          <t>Harpy</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. Townsfolk abilities yield false info. Each day, if no-one is executed, evil wins.</t>
+          <t>Each night, choose 2 players: tomorrow, the 1st player is mad that the 2nd is evil, or one or both might die.</t>
         </is>
       </c>
       <c r="E32" t="n">
         <v>1</v>
       </c>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="n">
-        <v>1</v>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>Yaggababble</t>
+          <t>Goblin</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>You start knowing a secret phrase. For each time you said it publicly today, a player might die.</t>
+          <t>If you publicly claim to be the Goblin when nominated &amp; are executed that day, your team wins.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" t="n">
-        <v>1</v>
-      </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>Zombuul</t>
+          <t>Mezepheles</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Each night*, if no-one died today, choose a player: they die. The 1st time you die, you live but register as dead.</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" t="inlineStr"/>
+          <t>You start knowing a secret word. The 1st good player to say this word becomes evil that night.</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>Politician</t>
+          <t>Marionette</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>If you were the player most responsible for your team losing, you change alignment &amp; win, even if dead.</t>
+          <t>You think you are a good character, but you are not. The Demon knows who you are. [You neighbor the Demon]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1200,17 +1184,17 @@
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>Ogre</t>
+          <t>Mastermind</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>No quoted ability text found</t>
+          <t>If the Demon dies by execution (ending the game), play for 1 more day. If a player is then executed, their team loses.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1221,17 +1205,17 @@
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>No Dashii</t>
+          <t>Poisoner</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. Your 2 Townsfolk neighbors are poisoned.</t>
+          <t>Each night, choose a player: they are poisoned tonight and tomorrow day.</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1244,17 +1228,17 @@
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kazali</t>
+          <t>Pit-Hag</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. [You choose which players are which Minions. -? to +? Outsiders]</t>
+          <t>Each night*, choose a player &amp; a character they become (if not in play). If a Demon is made, deaths tonight are arbitrary.</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1267,40 +1251,40 @@
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>Legion</t>
+          <t>Psychopath</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Each night*, a player might die. Executions fail if only evil voted. You register as a Minion too. [Most players are Legion]</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>1</v>
-      </c>
+          <t>Each day, before nominations, you may publicly choose a player: they die. If executed, you only die if you lose roshambo.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
       <c r="H39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>Lunatic</t>
+          <t>Evil Twin</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>You think you are a Demon, but you are not. The Demon knows who you are &amp; who you choose at night.</t>
+          <t>You &amp; an opposing player know each other. If the good player is executed, evil wins. Good can't win if you both live.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1311,17 +1295,17 @@
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>Lord of Typhon</t>
+          <t>Spy</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. [Evil characters are in a line. You are in the middle. +1 Minion. -? to +? Outsiders]</t>
+          <t>Each night, you see the Grimoire. You might register as good &amp; as a Townsfolk or Outsider, even if dead.</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1334,7 +1318,7 @@
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>Baron</t>
+          <t>Devil's Advocate</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1344,10 +1328,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>There are extra Outsiders in play. [+2 Outsiders]</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
+          <t>Each night, choose a living player (different to last night): if executed tomorrow, they don't die.</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
@@ -1355,7 +1341,7 @@
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Assassin</t>
+          <t>Summoner</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1365,20 +1351,18 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Once per game, at night*, choose a player: they die, even if for some reason they could not.</t>
+          <t>You get 3 bluffs. On the 3rd night, choose a player: they become an evil Demon of your choice. [No Demon]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
-        <v>1</v>
-      </c>
+      <c r="H43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>Boffin</t>
+          <t>Vizier</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1388,7 +1372,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>The Demon (even if drunk or poisoned) has a not-in-play good character's ability. You both know which.</t>
+          <t>All players know you are the Vizier. You cannot die during the day. If good voted, you may choose to execute immediately.</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1399,7 +1383,7 @@
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>Boomdandy</t>
+          <t>Widow</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1409,7 +1393,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>If you are executed, all but 3 players die. After a 10 to 1 countdown, the player with the most players pointing at them, dies.</t>
+          <t>On your first night, look at the Grimoire &amp; choose a player: they are poisoned. 1 good player knows a Widow is in play.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1420,7 +1404,7 @@
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cerenovus</t>
+          <t>Witch</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1430,7 +1414,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Each night, choose a player &amp; a good character: they are </t>
+          <t>Each night, choose a player: if they nominate tomorrow, they die. If just 3 players live, you lose this ability.</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -1443,7 +1427,7 @@
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>Fearmonger</t>
+          <t>Wizard</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1453,20 +1437,20 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Each night, choose a player: if you nominate &amp; execute them, their team loses. All players know if you choose a new player.</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, choose to make a wish. If granted, it might have a price &amp; leave a clue as to its nature.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>Godfather</t>
+          <t>Xaan</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1476,33 +1460,33 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>You start knowing which Outsiders are in play. If 1 died today, choose a player tonight: they die. [-1 or +1 Outsider]</t>
+          <t>On night X, all Townsfolk are poisoned until dusk. [X Outsiders]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="n">
-        <v>1</v>
-      </c>
+      <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>Goblin</t>
+          <t>Acrobat</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>If you publicly claim to be the Goblin when nominated &amp; are executed that day, your team wins.</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>Each night*, choose a player: if they are or become drunk or poisoned tonight, you die.</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>1</v>
+      </c>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
@@ -1510,40 +1494,40 @@
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>Harpy</t>
+          <t>Alsaahir</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Each night, choose 2 players: tomorrow, the 1st player is mad that the 2nd is evil, or one or both might die.</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
-        <v>1</v>
-      </c>
+          <t>Each day, if you publicly guess which players are Minion(s) and which are Demon(s), good wins.</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
+      <c r="G50" t="n">
+        <v>1</v>
+      </c>
       <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>Marionette</t>
+          <t>Alchemist</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>You think you are a good character, but you are not. The Demon knows who you are. [You neighbor the Demon]</t>
+          <t>You have a Minion ability. When using this, the Storyteller may prompt you to choose differently.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1554,66 +1538,66 @@
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>Mastermind</t>
+          <t>Amnesiac</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>If the Demon dies by execution (ending the game), play for 1 more day. If a player is then executed, their team loses.</t>
+          <t>You do not know what your ability is. Each day, privately guess what it is: you learn how accurate you are.</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>1</v>
+      </c>
       <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>Mezepheles</t>
+          <t>Artist</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>You start knowing a secret word. The 1st good player to say this word becomes evil that night.</t>
+          <t>Once per game, during the day, privately ask the Storyteller any yes/no question.</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" t="n">
-        <v>1</v>
-      </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" t="inlineStr">
         <is>
-          <t>Pit-Hag</t>
+          <t>Atheist</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Each night*, choose a player &amp; a character they become (if not in play). If a Demon is made, deaths tonight are arbitrary.</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
-        <v>1</v>
-      </c>
+          <t>The Storyteller can break the game rules, and if executed, good wins, even if you are dead. [No evil characters]</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
@@ -1621,20 +1605,22 @@
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>Plague Doctor</t>
+          <t>Balloonist</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>When you die, the Storyteller gains a Minion ability.</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
+          <t>Each night, you learn a player of a different character type than last night. [+0 or +1 Outsider]</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>1</v>
+      </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
@@ -1642,22 +1628,20 @@
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>Poisoner</t>
+          <t>Banshee</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Each night, choose a player: they are poisoned tonight and tomorrow day.</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
-        <v>1</v>
-      </c>
+          <t>No quoted ability text found</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
@@ -1665,40 +1649,38 @@
     <row r="57">
       <c r="B57" t="inlineStr">
         <is>
-          <t>Psychopath</t>
+          <t>Cannibal</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Each day, before nominations, you may publicly choose a player: they die. If executed, you only die if you lose roshambo.</t>
+          <t>You have the ability of the recently killed executee. If they are evil, you are poisoned until a good player dies by execution.</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
-      <c r="G57" t="n">
-        <v>1</v>
-      </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>Lil' Monsta</t>
+          <t>Organ Grinder</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Each night, Minions choose who babysits Lil' Monsta &amp; 'is the Demon'. Each night*, a player might die. [+1 Minion]</t>
+          <t>All players keep their eyes closed when voting and the vote tally is secret. Each night, choose if you are drunk until dusk.</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -1711,7 +1693,7 @@
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>Summoner</t>
+          <t>Scarlet Woman</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1721,7 +1703,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>You get 3 bluffs. On the 3rd night, choose a player: they become an evil Demon of your choice. [No Demon]</t>
+          <t>If there are 5 or more players alive &amp; the Demon dies, you become the Demon. (Travellers don't count)</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1732,20 +1714,22 @@
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>Evil Twin</t>
+          <t>Chambermaid</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>You &amp; an opposing player know each other. If the good player is executed, evil wins. Good can't win if you both live.</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
+          <t>Each night, choose 2 alive players (not yourself): you learn how many woke tonight due to their ability.</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
@@ -1753,22 +1737,20 @@
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>Spy</t>
+          <t>Choirboy</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Each night, you see the Grimoire. You might register as good &amp; as a Townsfolk or Outsider, even if dead.</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
-        <v>1</v>
-      </c>
+          <t>If the Demon kills the King, you learn which player is the Demon. [+the King]</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
@@ -1776,61 +1758,63 @@
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
-          <t>Devil's Advocate</t>
+          <t>Chef</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Each night, choose a living player (different to last night): if executed tomorrow, they don't die.</t>
-        </is>
-      </c>
-      <c r="E62" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" t="inlineStr"/>
+          <t>You start knowing how many pairs of evil players there are.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>Vizier</t>
+          <t>Clockmaker</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>All players know you are the Vizier. You cannot die during the day. If good voted, you may choose to execute immediately.</t>
+          <t>You start knowing how many steps from the Demon to its nearest Minion.</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>Wizard</t>
+          <t>Courtier</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Once per game, choose to make a wish. If granted, it might have a price &amp; leave a clue as to its nature.</t>
+          <t>Once per game, at night, choose a character: they are drunk for 3 nights &amp; 3 days.</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -1843,20 +1827,22 @@
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>Widow</t>
+          <t>Dreamer</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>On your first night, look at the Grimoire &amp; choose a player: they are poisoned. 1 good player knows a Widow is in play.</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr"/>
+          <t>Each night, choose a player (not yourself or Travellers): you learn 1 good &amp; 1 evil character, 1 of which is correct.</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>1</v>
+      </c>
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
@@ -1864,17 +1850,17 @@
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>Witch</t>
+          <t>Empath</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Each night, choose a player: if they nominate tomorrow, they die. If just 3 players live, you lose this ability.</t>
+          <t>Each night, you learn how many of your 2 alive neighbors are evil.</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -1887,7 +1873,7 @@
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
-          <t>Acrobat</t>
+          <t>Engineer</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1897,33 +1883,35 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: if they are or become drunk or poisoned tonight, you die.</t>
-        </is>
-      </c>
-      <c r="E67" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night, choose which Minions or which Demon is in play.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
+      <c r="H67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>Xaan</t>
+          <t>Exorcist</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>On night X, all Townsfolk are poisoned until dusk. [X Outsiders]</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr"/>
+          <t>Each night*, choose a player (different to last night): the Demon, if chosen, learns who you are then doesn't wake tonight.</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
@@ -1931,7 +1919,7 @@
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>Alchemist</t>
+          <t>Farmer</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1941,7 +1929,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>You have a Minion ability. When using this, the Storyteller may prompt you to choose differently.</t>
+          <t>When you die at night, an alive good player becomes a Farmer.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -1952,7 +1940,7 @@
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>Alsaahir</t>
+          <t>Fisherman</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1962,20 +1950,20 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Each day, if you publicly guess which players are Minion(s) and which are Demon(s), good wins.</t>
+          <t>Once per game, during the day, visit the Storyteller for some advice to help your team win.</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
-      <c r="G70" t="n">
-        <v>1</v>
-      </c>
-      <c r="H70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>Artist</t>
+          <t>Flowergirl</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1985,20 +1973,20 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Once per game, during the day, privately ask the Storyteller any yes/no question.</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr"/>
+          <t>Each night*, you learn if a Demon voted today.</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
-      <c r="H71" t="n">
-        <v>1</v>
-      </c>
+      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>Amnesiac</t>
+          <t>Fool</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2008,20 +1996,18 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>You do not know what your ability is. Each day, privately guess what it is: you learn how accurate you are.</t>
+          <t>The 1st time you die, you don't.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
-      <c r="G72" t="n">
-        <v>1</v>
-      </c>
+      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>Atheist</t>
+          <t>Gambler</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2031,10 +2017,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>The Storyteller can break the game rules, and if executed, good wins, even if you are dead. [No evil characters]</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr"/>
+          <t>Each night*, choose a player &amp; guess their character: if you guess wrong, you die.</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>1</v>
+      </c>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
@@ -2042,30 +2030,30 @@
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>Organ Grinder</t>
+          <t>Bounty Hunter</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>All players keep their eyes closed when voting and the vote tally is secret. Each night, choose if you are drunk until dusk.</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>1</v>
-      </c>
-      <c r="F74" t="inlineStr"/>
+          <t>You start knowing 1 evil player. If the player you know dies, you learn another evil player tonight. [1 Townsfolk is evil]</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="n">
+        <v>1</v>
+      </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>Balloonist</t>
+          <t>General</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2075,7 +2063,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Each night, you learn a player of a different character type than last night. [+0 or +1 Outsider]</t>
+          <t>Each night, you learn which alignment the Storyteller believes is winning: good, evil, or neither.</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2088,7 +2076,7 @@
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>Banshee</t>
+          <t>Gossip</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2098,18 +2086,20 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>No quoted ability text found</t>
+          <t>Each day, you may make a public statement. Tonight, if it was true, a player dies.</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
+      <c r="G76" t="n">
+        <v>1</v>
+      </c>
       <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>Cannibal</t>
+          <t>Grandmother</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2119,39 +2109,43 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>You have the ability of the recently killed executee. If they are evil, you are poisoned until a good player dies by execution.</t>
+          <t>You start knowing a good player &amp; their character. If the Demon kills them, you die too.</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>Scarlet Woman</t>
+          <t>Huntsman</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>If there are 5 or more players alive &amp; the Demon dies, you become the Demon. (Travellers don't count)</t>
+          <t>Once per game, at night, choose a living player: the Damsel, if chosen, becomes a not-in-play Townsfolk. [+the Damsel]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
+      <c r="H78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>Chambermaid</t>
+          <t>Innkeeper</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2161,7 +2155,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Each night, choose 2 alive players (not yourself): you learn how many woke tonight due to their ability.</t>
+          <t>Each night*, choose 2 players: they can't die tonight, but 1 is drunk until dusk.</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2174,7 +2168,7 @@
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>Choirboy</t>
+          <t>Investigator</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2184,18 +2178,20 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>If the Demon kills the King, you learn which player is the Demon. [+the King]</t>
+          <t>You start knowing that 1 of 2 players is a particular Minion.</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
-      <c r="F80" t="inlineStr"/>
+      <c r="F80" t="n">
+        <v>1</v>
+      </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>Clockmaker</t>
+          <t>Juggler</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2205,20 +2201,18 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>You start knowing how many steps from the Demon to its nearest Minion.</t>
+          <t>On your 1st day, publicly guess up to 5 players' characters. That night, you learn how many you got correct.</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
-      <c r="F81" t="n">
-        <v>1</v>
-      </c>
+      <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="B82" t="inlineStr">
         <is>
-          <t>Chef</t>
+          <t>Cult Leader</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2228,20 +2222,20 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>You start knowing how many pairs of evil players there are.</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night, you become the alignment of an alive neighbor. If all good players choose to join your cult, your team wins.</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>Courtier</t>
+          <t>King</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2251,20 +2245,20 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a character: they are drunk for 3 nights &amp; 3 days.</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr"/>
+          <t>Each night, if the dead equal or outnumber the living, you learn 1 alive character. The Demon knows you are the King.</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>1</v>
+      </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
-      <c r="H83" t="n">
-        <v>1</v>
-      </c>
+      <c r="H83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>Dreamer</t>
+          <t>Knight</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2274,20 +2268,20 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Each night, choose a player (not yourself or Travellers): you learn 1 good &amp; 1 evil character, 1 of which is correct.</t>
-        </is>
-      </c>
-      <c r="E84" t="n">
-        <v>1</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
+          <t>You start knowing 2 players that are not the Demon.</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="n">
+        <v>1</v>
+      </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
         <is>
-          <t>Empath</t>
+          <t>Librarian</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2297,20 +2291,20 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Each night, you learn how many of your 2 alive neighbors are evil.</t>
-        </is>
-      </c>
-      <c r="E85" t="n">
-        <v>1</v>
-      </c>
-      <c r="F85" t="inlineStr"/>
+          <t>You start knowing that 1 of 2 players is a particular Outsider. (Or that zero are in play.)</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="n">
+        <v>1</v>
+      </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>Exorcist</t>
+          <t>Lycanthrope</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2320,7 +2314,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Each night*, choose a player (different to last night): the Demon, if chosen, learns who you are then doesn't wake tonight.</t>
+          <t>Each night*, choose an alive player. If good, they die &amp; the Demon doesn’t kill tonight. One good player registers as evil.</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2333,7 +2327,7 @@
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>Engineer</t>
+          <t>Magician</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2343,20 +2337,18 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose which Minions or which Demon is in play.</t>
+          <t>The Demon thinks you are a Minion. Minions think you are a Demon.</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
-      <c r="H87" t="n">
-        <v>1</v>
-      </c>
+      <c r="H87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>Farmer</t>
+          <t>Mathematician</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2366,10 +2358,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>When you die at night, an alive good player becomes a Farmer.</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr"/>
+          <t>Each night, you learn how many players' abilities worked abnormally (since dawn) due to another character's ability.</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>1</v>
+      </c>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
@@ -2377,7 +2371,7 @@
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>Fisherman</t>
+          <t>Mayor</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2387,20 +2381,18 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Once per game, during the day, visit the Storyteller for some advice to help your team win.</t>
+          <t>If only 3 players live &amp; no execution occurs, your team wins. If you die at night, another player might die instead.</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
-      <c r="H89" t="n">
-        <v>1</v>
-      </c>
+      <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>Flowergirl</t>
+          <t>Fortune Teller</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2410,7 +2402,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Each night*, you learn if a Demon voted today.</t>
+          <t>Each night, choose 2 players: you learn if either is a Demon. There is a good player that registers as a Demon to you.</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -2423,7 +2415,7 @@
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>Fool</t>
+          <t>Minstrel</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2433,7 +2425,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>The 1st time you die, you don't.</t>
+          <t>When a Minion dies by execution, all other players (except Travellers) are drunk until dusk tomorrow.</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -2444,7 +2436,7 @@
     <row r="92">
       <c r="B92" t="inlineStr">
         <is>
-          <t>Bounty Hunter</t>
+          <t>Monk</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2454,20 +2446,20 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>You start knowing 1 evil player. If the player you know dies, you learn another evil player tonight. [1 Townsfolk is evil]</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, choose a player (not yourself): they are safe from the Demon tonight.</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>1</v>
+      </c>
+      <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>Gambler</t>
+          <t>Nightwatchman</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2477,20 +2469,20 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Each night*, choose a player &amp; guess their character: if you guess wrong, you die.</t>
-        </is>
-      </c>
-      <c r="E93" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night, choose a player: they learn you are the Nightwatchman.</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr"/>
+      <c r="H93" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Oracle</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2500,7 +2492,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Each night, you learn which alignment the Storyteller believes is winning: good, evil, or neither.</t>
+          <t>Each night*, you learn how many dead players are evil.</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -2513,7 +2505,7 @@
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>Gossip</t>
+          <t>Noble</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2523,20 +2515,20 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Each day, you may make a public statement. Tonight, if it was true, a player dies.</t>
+          <t>You start knowing 3 players, 1 and only 1 of which is evil.</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="n">
-        <v>1</v>
-      </c>
+      <c r="F95" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>Grandmother</t>
+          <t>High Priestess</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2546,20 +2538,20 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>You start knowing a good player &amp; their character. If the Demon kills them, you die too.</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night, learn which player the Storyteller believes you should talk to most.</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="B97" t="inlineStr">
         <is>
-          <t>Innkeeper</t>
+          <t>Pacifist</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2569,12 +2561,10 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Each night*, choose 2 players: they can't die tonight, but 1 is drunk until dusk.</t>
-        </is>
-      </c>
-      <c r="E97" t="n">
-        <v>1</v>
-      </c>
+          <t>Executed good players might not die.</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
@@ -2582,7 +2572,7 @@
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>Huntsman</t>
+          <t>Philosopher</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2592,7 +2582,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a living player: the Damsel, if chosen, becomes a not-in-play Townsfolk. [+the Damsel]</t>
+          <t>Once per game, at night, choose a good character: gain that ability. If this character is in play, they are drunk.</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -2605,7 +2595,7 @@
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
-          <t>Investigator</t>
+          <t>Pixie</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2615,7 +2605,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>You start knowing that 1 of 2 players is a particular Minion.</t>
+          <t>You start knowing 1 in-play Townsfolk. If you were mad that you were this character, you gain their ability when they die.</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -2628,7 +2618,7 @@
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>Juggler</t>
+          <t>Preacher</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2638,10 +2628,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>On your 1st day, publicly guess up to 5 players' characters. That night, you learn how many you got correct.</t>
-        </is>
-      </c>
-      <c r="E100" t="inlineStr"/>
+          <t>Each night, choose a player: a Minion, if chosen, learns this. All chosen Minions have no ability.</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>1</v>
+      </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
@@ -2649,7 +2641,7 @@
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>Knight</t>
+          <t>Professor</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2659,20 +2651,20 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>You start knowing 2 players that are not the Demon.</t>
+          <t>Once per game, at night*, choose a dead player: if they are a Townsfolk, they are resurrected.</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>
-      <c r="F101" t="n">
-        <v>1</v>
-      </c>
+      <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
+      <c r="H101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Sage</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2682,12 +2674,10 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Each night, if the dead equal or outnumber the living, you learn 1 alive character. The Demon knows you are the King.</t>
-        </is>
-      </c>
-      <c r="E102" t="n">
-        <v>1</v>
-      </c>
+          <t>If the Demon kills you, you learn that it is 1 of 2 players.</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr"/>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
@@ -2695,7 +2685,7 @@
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>Cult Leader</t>
+          <t>Ravenkeeper</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2705,12 +2695,10 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Each night, you become the alignment of an alive neighbor. If all good players choose to join your cult, your team wins.</t>
-        </is>
-      </c>
-      <c r="E103" t="n">
-        <v>1</v>
-      </c>
+          <t>If you die at night, you are woken to choose a player: you learn their character.</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
@@ -2718,7 +2706,7 @@
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>Lycanthrope</t>
+          <t>Sailor</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2728,7 +2716,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Each night*, choose an alive player. If good, they die &amp; the Demon doesn’t kill tonight. One good player registers as evil.</t>
+          <t>Each night, choose an alive player: either you or they are drunk until dusk. You can't die.</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -2741,7 +2729,7 @@
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>Librarian</t>
+          <t>Savant</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2751,20 +2739,20 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>You start knowing that 1 of 2 players is a particular Outsider. (Or that zero are in play.)</t>
+          <t>Each day, you may visit the Storyteller to learn 2 things in private: 1 is true &amp; 1 is false.</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
-      <c r="F105" t="n">
-        <v>1</v>
-      </c>
-      <c r="G105" t="inlineStr"/>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="n">
+        <v>1</v>
+      </c>
       <c r="H105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>Magician</t>
+          <t>Seamstress</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2774,18 +2762,20 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>The Demon thinks you are a Minion. Minions think you are a Demon.</t>
+          <t>Once per game, at night, choose 2 players (not yourself): you learn if they are the same alignment.</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
+      <c r="H106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
       <c r="B107" t="inlineStr">
         <is>
-          <t>Mathematician</t>
+          <t>Shugenja</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2795,20 +2785,20 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Each night, you learn how many players' abilities worked abnormally (since dawn) due to another character's ability.</t>
-        </is>
-      </c>
-      <c r="E107" t="n">
-        <v>1</v>
-      </c>
-      <c r="F107" t="inlineStr"/>
+          <t>You start knowing if your closest evil player is clockwise or anti-clockwise. If equidistant, this info is arbitrary.</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="n">
+        <v>1</v>
+      </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="B108" t="inlineStr">
         <is>
-          <t>Mayor</t>
+          <t>Slayer</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2818,18 +2808,20 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>If only 3 players live &amp; no execution occurs, your team wins. If you die at night, another player might die instead.</t>
+          <t>Once per game, during the day, publicly choose a player: if they are the Demon, they die.</t>
         </is>
       </c>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
-      <c r="H108" t="inlineStr"/>
+      <c r="H108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>Minstrel</t>
+          <t>Soldier</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2839,7 +2831,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>When a Minion dies by execution, all other players (except Travellers) are drunk until dusk tomorrow.</t>
+          <t>You are safe from the Demon.</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
@@ -2850,7 +2842,7 @@
     <row r="110">
       <c r="B110" t="inlineStr">
         <is>
-          <t>Monk</t>
+          <t>Steward</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2860,20 +2852,20 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Each night*, choose a player (not yourself): they are safe from the Demon tonight.</t>
-        </is>
-      </c>
-      <c r="E110" t="n">
-        <v>1</v>
-      </c>
-      <c r="F110" t="inlineStr"/>
+          <t>You start knowing 1 good player.</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="n">
+        <v>1</v>
+      </c>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="B111" t="inlineStr">
         <is>
-          <t>Nightwatchman</t>
+          <t>Undertaker</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2883,20 +2875,20 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a player: they learn you are the Nightwatchman.</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr"/>
+          <t>Each night*, you learn which character died by execution today.</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>1</v>
+      </c>
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
-      <c r="H111" t="n">
-        <v>1</v>
-      </c>
+      <c r="H111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="B112" t="inlineStr">
         <is>
-          <t>Fortune Teller</t>
+          <t>Virgin</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2906,12 +2898,10 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Each night, choose 2 players: you learn if either is a Demon. There is a good player that registers as a Demon to you.</t>
-        </is>
-      </c>
-      <c r="E112" t="n">
-        <v>1</v>
-      </c>
+          <t>The 1st time you are nominated, if the nominator is a Townsfolk, they are executed immediately.</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
@@ -2919,7 +2909,7 @@
     <row r="113">
       <c r="B113" t="inlineStr">
         <is>
-          <t>Oracle</t>
+          <t>Washerwoman</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2929,43 +2919,43 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Each night*, you learn how many dead players are evil.</t>
-        </is>
-      </c>
-      <c r="E113" t="n">
-        <v>1</v>
-      </c>
-      <c r="F113" t="inlineStr"/>
+          <t>You start knowing that 1 of 2 players is a particular Townsfolk.</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="n">
+        <v>1</v>
+      </c>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="B114" t="inlineStr">
         <is>
-          <t>Noble</t>
+          <t>Al-Hadikhia</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>You start knowing 3 players, 1 and only 1 of which is evil.</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr"/>
-      <c r="F114" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, you may choose 3 players (all players learn who): each silently chooses to live or die, but if all live, all die.</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>1</v>
+      </c>
+      <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="B115" t="inlineStr">
         <is>
-          <t>Pacifist</t>
+          <t>Poppy Grower</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2975,7 +2965,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Executed good players might not die.</t>
+          <t>Minions &amp; Demons do not know each other. If you die, they learn who each other are that night.</t>
         </is>
       </c>
       <c r="E115" t="inlineStr"/>
@@ -2986,68 +2976,66 @@
     <row r="116">
       <c r="B116" t="inlineStr">
         <is>
-          <t>Philosopher</t>
+          <t>Kazali</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a good character: gain that ability. If this character is in play, they are drunk.</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. [You choose which players are which Minions. -? to +? Outsiders]</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>1</v>
+      </c>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
-      <c r="H116" t="n">
-        <v>1</v>
-      </c>
+      <c r="H116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="B117" t="inlineStr">
         <is>
-          <t>Pixie</t>
+          <t>Imp</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>You start knowing 1 in-play Townsfolk. If you were mad that you were this character, you gain their ability when they die.</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr"/>
-      <c r="F117" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, choose a player: they die. If you kill yourself this way, a Minion becomes the Imp.</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>1</v>
+      </c>
+      <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="B118" t="inlineStr">
         <is>
-          <t>High Priestess</t>
+          <t>Leviathan</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Each night, learn which player the Storyteller believes you should talk to most.</t>
-        </is>
-      </c>
-      <c r="E118" t="n">
-        <v>1</v>
-      </c>
+          <t>If more than 1 good player is executed, evil wins. All players know you are in play. After day 5, evil wins.</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
@@ -3055,17 +3043,17 @@
     <row r="119">
       <c r="B119" t="inlineStr">
         <is>
-          <t>Preacher</t>
+          <t>Legion</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Each night, choose a player: a Minion, if chosen, learns this. All chosen Minions have no ability.</t>
+          <t>Each night*, a player might die. Executions fail if only evil voted. You register as a Minion too. [Most players are Legion]</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3078,30 +3066,32 @@
     <row r="120">
       <c r="B120" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Lleech</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Once per game, at night*, choose a dead player: if they are a Townsfolk, they are resurrected.</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr"/>
-      <c r="F120" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. You start by choosing a player: they are poisoned. You die if &amp; only if they are dead.</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>1</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1</v>
+      </c>
       <c r="G120" t="inlineStr"/>
-      <c r="H120" t="n">
-        <v>1</v>
-      </c>
+      <c r="H120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="B121" t="inlineStr">
         <is>
-          <t>Ravenkeeper</t>
+          <t>Snake Charmer</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3111,10 +3101,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>If you die at night, you are woken to choose a player: you learn their character.</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr"/>
+          <t>Each night, choose an alive player: a chosen Demon swaps characters &amp; alignments with you &amp; is then poisoned.</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>1</v>
+      </c>
       <c r="F121" t="inlineStr"/>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr"/>
@@ -3122,17 +3114,17 @@
     <row r="122">
       <c r="B122" t="inlineStr">
         <is>
-          <t>Sailor</t>
+          <t>Ojo</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Each night, choose an alive player: either you or they are drunk until dusk. You can't die.</t>
+          <t>Each night*, choose a character: they die. If they are not in play, the Storyteller chooses who dies.</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -3145,7 +3137,7 @@
     <row r="123">
       <c r="B123" t="inlineStr">
         <is>
-          <t>Sage</t>
+          <t>Tea Lady</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3155,7 +3147,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>If the Demon kills you, you learn that it is 1 of 2 players.</t>
+          <t>If both your alive neighbors are good, they can't die.</t>
         </is>
       </c>
       <c r="E123" t="inlineStr"/>
@@ -3166,53 +3158,53 @@
     <row r="124">
       <c r="B124" t="inlineStr">
         <is>
-          <t>Savant</t>
+          <t>Po</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Each day, you may visit the Storyteller to learn 2 things in private: 1 is true &amp; 1 is false.</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr"/>
+          <t>Each night*, you may choose a player: they die. If your last choice was no-one, choose 3 players tonight.</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>1</v>
+      </c>
       <c r="F124" t="inlineStr"/>
-      <c r="G124" t="n">
-        <v>1</v>
-      </c>
+      <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="B125" t="inlineStr">
         <is>
-          <t>Seamstress</t>
+          <t>Pukka</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose 2 players (not yourself): you learn if they are the same alignment.</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr"/>
+          <t>Each night, choose a player: they are poisoned. The previously poisoned player dies then becomes healthy.</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>1</v>
+      </c>
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
-      <c r="H125" t="n">
-        <v>1</v>
-      </c>
+      <c r="H125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="B126" t="inlineStr">
         <is>
-          <t>Shugenja</t>
+          <t>Town Crier</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3222,43 +3214,41 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>You start knowing if your closest evil player is clockwise or anti-clockwise. If equidistant, this info is arbitrary.</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr"/>
-      <c r="F126" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, you learn if a Minion nominated today.</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>1</v>
+      </c>
+      <c r="F126" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="B127" t="inlineStr">
         <is>
-          <t>Slayer</t>
+          <t>Riot</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Once per game, during the day, publicly choose a player: if they are the Demon, they die.</t>
+          <t>On day 3, Minions become Riot &amp; nominees die but nominate an alive player immediately. This must happen.</t>
         </is>
       </c>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
       <c r="G127" t="inlineStr"/>
-      <c r="H127" t="n">
-        <v>1</v>
-      </c>
+      <c r="H127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="B128" t="inlineStr">
         <is>
-          <t>Soldier</t>
+          <t>Village Idiot</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3268,10 +3258,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>You are safe from the Demon.</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr"/>
+          <t>Each night, choose a player: you learn their alignment. [+0 to +2 Village Idiots. 1 of the extras is drunk]</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>1</v>
+      </c>
       <c r="F128" t="inlineStr"/>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
@@ -3279,43 +3271,45 @@
     <row r="129">
       <c r="B129" t="inlineStr">
         <is>
-          <t>Steward</t>
+          <t>Shabaloth</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>You start knowing 1 good player.</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr"/>
-      <c r="F129" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, choose 2 players: they die. A dead player you chose last night might be regurgitated.</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="B130" t="inlineStr">
         <is>
-          <t>Virgin</t>
+          <t>Vigormortis</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>The 1st time you are nominated, if the nominator is a Townsfolk, they are executed immediately.</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. Minions you kill keep their ability &amp; poison 1 Townsfolk neighbor. [-1 Outsider]</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>1</v>
+      </c>
       <c r="F130" t="inlineStr"/>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr"/>
@@ -3323,66 +3317,70 @@
     <row r="131">
       <c r="B131" t="inlineStr">
         <is>
-          <t>Undertaker</t>
+          <t>Yaggababble</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Each night*, you learn which character died by execution today.</t>
-        </is>
-      </c>
-      <c r="E131" t="n">
-        <v>1</v>
-      </c>
-      <c r="F131" t="inlineStr"/>
+          <t>You start knowing a secret phrase. For each time you said it publicly today, a player might die.</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="n">
+        <v>1</v>
+      </c>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="B132" t="inlineStr">
         <is>
-          <t>Washerwoman</t>
+          <t>Vortox</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>You start knowing that 1 of 2 players is a particular Townsfolk.</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr"/>
-      <c r="F132" t="n">
-        <v>1</v>
-      </c>
-      <c r="G132" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. Townsfolk abilities yield false info. Each day, if no-one is executed, evil wins.</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>1</v>
+      </c>
+      <c r="F132" t="inlineStr"/>
+      <c r="G132" t="n">
+        <v>1</v>
+      </c>
       <c r="H132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="B133" t="inlineStr">
         <is>
-          <t>Poppy Grower</t>
+          <t>Fang Gu</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Minions &amp; Demons do not know each other. If you die, they learn who each other are that night.</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. The 1st Outsider this kills becomes an evil Fang Gu &amp; you die instead. [+1 Outsider]</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
@@ -3390,17 +3388,17 @@
     <row r="134">
       <c r="B134" t="inlineStr">
         <is>
-          <t>Snake Charmer</t>
+          <t>Lil' Monsta</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Each night, choose an alive player: a chosen Demon swaps characters &amp; alignments with you &amp; is then poisoned.</t>
+          <t>Each night, Minions choose who babysits Lil' Monsta &amp; 'is the Demon'. Each night*, a player might die. [+1 Minion]</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -3413,17 +3411,17 @@
     <row r="135">
       <c r="B135" t="inlineStr">
         <is>
-          <t>Town Crier</t>
+          <t>Zombuul</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Each night*, you learn if a Minion nominated today.</t>
+          <t>Each night*, if no-one died today, choose a player: they die. The 1st time you die, you live but register as dead.</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -3436,20 +3434,22 @@
     <row r="136">
       <c r="B136" t="inlineStr">
         <is>
-          <t>Tea Lady</t>
+          <t>Lord of Typhon</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>If both your alive neighbors are good, they can't die.</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. [Evil characters are in a line. You are in the middle. +1 Minion. -? to +? Outsiders]</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
       <c r="F136" t="inlineStr"/>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="inlineStr"/>
@@ -3457,17 +3457,17 @@
     <row r="137">
       <c r="B137" t="inlineStr">
         <is>
-          <t>Village Idiot</t>
+          <t>No Dashii</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Each night, choose a player: you learn their alignment. [+0 to +2 Village Idiots. 1 of the extras is drunk]</t>
+          <t>Each night*, choose a player: they die. Your 2 Townsfolk neighbors are poisoned.</t>
         </is>
       </c>
       <c r="E137" t="n">

</xml_diff>

<commit_message>
use custom sorting for json uploader
</commit_message>
<xml_diff>
--- a/botc_character_list.xlsx
+++ b/botc_character_list.xlsx
@@ -473,7 +473,7 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Butler</t>
+          <t>Barber</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -483,12 +483,10 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Each night, choose a player (not yourself): tomorrow, you may only vote if they are voting too.</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
+          <t>If you died today or tonight, the Demon may choose 2 players (not another Demon) to swap characters.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -496,7 +494,7 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Drunk</t>
+          <t>Butler</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -506,10 +504,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>You do not know you are the Drunk. You think you are a Townsfolk character, but you are not.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>Each night, choose a player (not yourself): tomorrow, you may only vote if they are voting too.</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -517,7 +517,7 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Barber</t>
+          <t>Damsel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>If you died today or tonight, the Demon may choose 2 players (not another Demon) to swap characters.</t>
+          <t>All Minions know a Damsel is in play. If a Minion publicly guesses you (once), your team loses.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -538,7 +538,7 @@
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>Damsel</t>
+          <t>Drunk</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>All Minions know a Damsel is in play. If a Minion publicly guesses you (once), your team loses.</t>
+          <t>You do not know you are the Drunk. You think you are a Townsfolk character, but you are not.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -559,7 +559,7 @@
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>Golem</t>
+          <t>Tinker</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -569,33 +569,33 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>You may only nominate once per game. When you do, if the nominee is not the Demon, they die.</t>
+          <t>You might die at any time.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hatter</t>
+          <t>Fearmonger</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>If you died today or tonight, the Minion &amp; Demon players may choose new Minion &amp; Demon characters to be.</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>Each night, choose a player: if you nominate &amp; execute them, their team loses. All players know if you choose a new player.</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -603,28 +603,30 @@
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Saint</t>
+          <t>Assassin</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>If you die by execution, your team loses.</t>
+          <t>Once per game, at night*, choose a player: they die, even if for some reason they could not.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>Klutz</t>
+          <t>Sweetheart</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -634,7 +636,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>When you learn that you died, publicly choose 1 alive player: if they are evil, your team loses.</t>
+          <t>When you die, 1 player is drunk from now on.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -645,7 +647,7 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Goon</t>
+          <t>Golem</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -655,30 +657,30 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Each night, the 1st player to choose you with their ability is drunk until dusk. You become their alignment.</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>1</v>
-      </c>
+          <t>You may only nominate once per game. When you do, if the nominee is not the Demon, they die.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Boffin</t>
+          <t>Klutz</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>The Demon (even if drunk or poisoned) has a not-in-play good character's ability. You both know which.</t>
+          <t>When you learn that you died, publicly choose 1 alive player: if they are evil, your team loses.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -689,7 +691,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Heretic</t>
+          <t>Goon</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -699,10 +701,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Whoever wins, loses &amp; whoever loses, wins, even if you are dead.</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>Each night, the 1st player to choose you with their ability is drunk until dusk. You become their alignment.</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
@@ -710,17 +714,17 @@
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>Baron</t>
+          <t>Moonchild</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>There are extra Outsiders in play. [+2 Outsiders]</t>
+          <t>When you learn that you died, publicly choose 1 alive player. Tonight, if it was a good player, they die.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -731,7 +735,7 @@
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mutant</t>
+          <t>Puzzlemaster</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -741,7 +745,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">If you are </t>
+          <t>1 player is drunk, even if you die. If you guess (once) who it is, learn the Demon player, but guess wrong &amp; get false info.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -752,7 +756,7 @@
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>Puzzlemaster</t>
+          <t>Saint</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -762,7 +766,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1 player is drunk, even if you die. If you guess (once) who it is, learn the Demon player, but guess wrong &amp; get false info.</t>
+          <t>If you die by execution, your team loses.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -794,7 +798,7 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>Recluse</t>
+          <t>Heretic</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -804,7 +808,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>You might register as evil &amp; as a Minion or Demon, even if dead.</t>
+          <t>Whoever wins, loses &amp; whoever loses, wins, even if you are dead.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -815,7 +819,7 @@
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tinker</t>
+          <t>Lunatic</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -825,7 +829,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>You might die at any time.</t>
+          <t>You think you are a Demon, but you are not. The Demon knows who you are &amp; who you choose at night.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -836,20 +840,22 @@
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ogre</t>
+          <t>Cerenovus</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>No quoted ability text found</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t xml:space="preserve">Each night, choose a player &amp; a good character: they are </t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
@@ -857,7 +863,7 @@
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lunatic</t>
+          <t>Recluse</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -867,7 +873,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>You think you are a Demon, but you are not. The Demon knows who you are &amp; who you choose at night.</t>
+          <t>You might register as evil &amp; as a Minion or Demon, even if dead.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -878,7 +884,7 @@
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cerenovus</t>
+          <t>Baron</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -888,12 +894,10 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Each night, choose a player &amp; a good character: they are </t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
+          <t>There are extra Outsiders in play. [+2 Outsiders]</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
@@ -901,30 +905,28 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>Assassin</t>
+          <t>Mutant</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Once per game, at night*, choose a player: they die, even if for some reason they could not.</t>
+          <t xml:space="preserve">If you are </t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
-      <c r="H23" t="n">
-        <v>1</v>
-      </c>
+      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sweetheart</t>
+          <t>Politician</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -934,7 +936,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>When you die, 1 player is drunk from now on.</t>
+          <t>If you were the player most responsible for your team losing, you change alignment &amp; win, even if dead.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -945,7 +947,7 @@
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fearmonger</t>
+          <t>Boomdandy</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -955,12 +957,10 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Each night, choose a player: if you nominate &amp; execute them, their team loses. All players know if you choose a new player.</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>1</v>
-      </c>
+          <t>If you are executed, all but 3 players die. After a 10 to 1 countdown, the player with the most players pointing at them, dies.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
@@ -968,17 +968,17 @@
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>Zealot</t>
+          <t>Boffin</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>If there are 5 or more players alive, you must vote for every nomination.</t>
+          <t>The Demon (even if drunk or poisoned) has a not-in-play good character's ability. You both know which.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -989,17 +989,17 @@
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>Boomdandy</t>
+          <t>Ogre</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>If you are executed, all but 3 players die. After a 10 to 1 countdown, the player with the most players pointing at them, dies.</t>
+          <t>No quoted ability text found</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1010,7 +1010,7 @@
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>Moonchild</t>
+          <t>Zealot</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>When you learn that you died, publicly choose 1 alive player. Tonight, if it was a good player, they die.</t>
+          <t>If there are 5 or more players alive, you must vote for every nomination.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1031,7 +1031,7 @@
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>Politician</t>
+          <t>Hatter</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>If you were the player most responsible for your team losing, you change alignment &amp; win, even if dead.</t>
+          <t>If you died today or tonight, the Minion &amp; Demon players may choose new Minion &amp; Demon characters to be.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1052,17 +1052,17 @@
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>Plague Doctor</t>
+          <t>Goblin</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Outsiders</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>When you die, the Storyteller gains a Minion ability.</t>
+          <t>If you publicly claim to be the Goblin when nominated &amp; are executed that day, your team wins.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1119,7 +1119,7 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>Goblin</t>
+          <t>Marionette</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1129,7 +1129,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>If you publicly claim to be the Goblin when nominated &amp; are executed that day, your team wins.</t>
+          <t>You think you are a good character, but you are not. The Demon knows who you are. [You neighbor the Demon]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1140,7 +1140,7 @@
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mezepheles</t>
+          <t>Mastermind</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1150,20 +1150,18 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>You start knowing a secret word. The 1st good player to say this word becomes evil that night.</t>
+          <t>If the Demon dies by execution (ending the game), play for 1 more day. If a player is then executed, their team loses.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="n">
-        <v>1</v>
-      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>Marionette</t>
+          <t>Devil's Advocate</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1173,10 +1171,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>You think you are a good character, but you are not. The Demon knows who you are. [You neighbor the Demon]</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
+          <t>Each night, choose a living player (different to last night): if executed tomorrow, they don't die.</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
@@ -1184,7 +1184,7 @@
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mastermind</t>
+          <t>Mezepheles</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1194,18 +1194,20 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>If the Demon dies by execution (ending the game), play for 1 more day. If a player is then executed, their team loses.</t>
+          <t>You start knowing a secret word. The 1st good player to say this word becomes evil that night.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>Poisoner</t>
+          <t>Evil Twin</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1215,12 +1217,10 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Each night, choose a player: they are poisoned tonight and tomorrow day.</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>1</v>
-      </c>
+          <t>You &amp; an opposing player know each other. If the good player is executed, evil wins. Good can't win if you both live.</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
@@ -1251,7 +1251,7 @@
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>Psychopath</t>
+          <t>Poisoner</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1261,30 +1261,30 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Each day, before nominations, you may publicly choose a player: they die. If executed, you only die if you lose roshambo.</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>Each night, choose a player: they are poisoned tonight and tomorrow day.</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="n">
-        <v>1</v>
-      </c>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>Evil Twin</t>
+          <t>Plague Doctor</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Outsiders</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>You &amp; an opposing player know each other. If the good player is executed, evil wins. Good can't win if you both live.</t>
+          <t>When you die, the Storyteller gains a Minion ability.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1318,7 +1318,7 @@
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>Devil's Advocate</t>
+          <t>Psychopath</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1328,20 +1328,20 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Each night, choose a living player (different to last night): if executed tomorrow, they don't die.</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>1</v>
-      </c>
+          <t>Each day, before nominations, you may publicly choose a player: they die. If executed, you only die if you lose roshambo.</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
       <c r="H42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Summoner</t>
+          <t>Vizier</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>You get 3 bluffs. On the 3rd night, choose a player: they become an evil Demon of your choice. [No Demon]</t>
+          <t>All players know you are the Vizier. You cannot die during the day. If good voted, you may choose to execute immediately.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -1362,7 +1362,7 @@
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>Vizier</t>
+          <t>Witch</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1372,10 +1372,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>All players know you are the Vizier. You cannot die during the day. If good voted, you may choose to execute immediately.</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
+          <t>Each night, choose a player: if they nominate tomorrow, they die. If just 3 players live, you lose this ability.</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
@@ -1383,7 +1385,7 @@
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>Widow</t>
+          <t>Wizard</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1393,18 +1395,20 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>On your first night, look at the Grimoire &amp; choose a player: they are poisoned. 1 good player knows a Widow is in play.</t>
+          <t>Once per game, choose to make a wish. If granted, it might have a price &amp; leave a clue as to its nature.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>Witch</t>
+          <t>Xaan</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1414,12 +1418,10 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Each night, choose a player: if they nominate tomorrow, they die. If just 3 players live, you lose this ability.</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
-        <v>1</v>
-      </c>
+          <t>On night X, all Townsfolk are poisoned until dusk. [X Outsiders]</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
@@ -1427,43 +1429,45 @@
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>Wizard</t>
+          <t>Al-Hadikhia</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Once per game, choose to make a wish. If granted, it might have a price &amp; leave a clue as to its nature.</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
+          <t>Each night*, you may choose 3 players (all players learn who): each silently chooses to live or die, but if all live, all die.</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
-      <c r="H47" t="n">
-        <v>1</v>
-      </c>
+      <c r="H47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>Xaan</t>
+          <t>Imp</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>On night X, all Townsfolk are poisoned until dusk. [X Outsiders]</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. If you kill yourself this way, a Minion becomes the Imp.</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>1</v>
+      </c>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
@@ -1471,17 +1475,17 @@
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>Acrobat</t>
+          <t>Kazali</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: if they are or become drunk or poisoned tonight, you die.</t>
+          <t>Each night*, choose a player: they die. [You choose which players are which Minions. -? to +? Outsiders]</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1494,40 +1498,40 @@
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>Alsaahir</t>
+          <t>Legion</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Each day, if you publicly guess which players are Minion(s) and which are Demon(s), good wins.</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr"/>
+          <t>Each night*, a player might die. Executions fail if only evil voted. You register as a Minion too. [Most players are Legion]</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="n">
-        <v>1</v>
-      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>Alchemist</t>
+          <t>Leviathan</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>You have a Minion ability. When using this, the Storyteller may prompt you to choose differently.</t>
+          <t>If more than 1 good player is executed, evil wins. All players know you are in play. After day 5, evil wins.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1538,63 +1542,65 @@
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>Amnesiac</t>
+          <t>Organ Grinder</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>You do not know what your ability is. Each day, privately guess what it is: you learn how accurate you are.</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr"/>
+          <t>All players keep their eyes closed when voting and the vote tally is secret. Each night, choose if you are drunk until dusk.</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
       <c r="F52" t="inlineStr"/>
-      <c r="G52" t="n">
-        <v>1</v>
-      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>Artist</t>
+          <t>Lleech</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Once per game, during the day, privately ask the Storyteller any yes/no question.</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. You start by choosing a player: they are poisoned. You die if &amp; only if they are dead.</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1</v>
+      </c>
       <c r="G53" t="inlineStr"/>
-      <c r="H53" t="n">
-        <v>1</v>
-      </c>
+      <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="B54" t="inlineStr">
         <is>
-          <t>Atheist</t>
+          <t>Scarlet Woman</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>The Storyteller can break the game rules, and if executed, good wins, even if you are dead. [No evil characters]</t>
+          <t>If there are 5 or more players alive &amp; the Demon dies, you become the Demon. (Travellers don't count)</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -1605,17 +1611,17 @@
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>Balloonist</t>
+          <t>Ojo</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Each night, you learn a player of a different character type than last night. [+0 or +1 Outsider]</t>
+          <t>Each night*, choose a character: they die. If they are not in play, the Storyteller chooses who dies.</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1628,20 +1634,22 @@
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>Banshee</t>
+          <t>Pukka</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>No quoted ability text found</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>Each night, choose a player: they are poisoned. The previously poisoned player dies then becomes healthy.</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
@@ -1649,20 +1657,22 @@
     <row r="57">
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cannibal</t>
+          <t>Po</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>You have the ability of the recently killed executee. If they are evil, you are poisoned until a good player dies by execution.</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr"/>
+          <t>Each night*, you may choose a player: they die. If your last choice was no-one, choose 3 players tonight.</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>1</v>
+      </c>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
@@ -1670,7 +1680,7 @@
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>Organ Grinder</t>
+          <t>Widow</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1680,12 +1690,10 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>All players keep their eyes closed when voting and the vote tally is secret. Each night, choose if you are drunk until dusk.</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
-        <v>1</v>
-      </c>
+          <t>On your first night, look at the Grimoire &amp; choose a player: they are poisoned. 1 good player knows a Widow is in play.</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
@@ -1693,17 +1701,17 @@
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>Scarlet Woman</t>
+          <t>Riot</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Minions</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>If there are 5 or more players alive &amp; the Demon dies, you become the Demon. (Travellers don't count)</t>
+          <t>On day 3, Minions become Riot &amp; nominees die but nominate an alive player immediately. This must happen.</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1714,17 +1722,17 @@
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>Chambermaid</t>
+          <t>Shabaloth</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Each night, choose 2 alive players (not yourself): you learn how many woke tonight due to their ability.</t>
+          <t>Each night*, choose 2 players: they die. A dead player you chose last night might be regurgitated.</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -1737,20 +1745,22 @@
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>Choirboy</t>
+          <t>Vigormortis</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>If the Demon kills the King, you learn which player is the Demon. [+the King]</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. Minions you kill keep their ability &amp; poison 1 Townsfolk neighbor. [-1 Outsider]</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
@@ -1758,86 +1768,86 @@
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
-          <t>Chef</t>
+          <t>Summoner</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Minions</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>You start knowing how many pairs of evil players there are.</t>
+          <t>You get 3 bluffs. On the 3rd night, choose a player: they become an evil Demon of your choice. [No Demon]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" t="n">
-        <v>1</v>
-      </c>
+      <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>Clockmaker</t>
+          <t>Vortox</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>You start knowing how many steps from the Demon to its nearest Minion.</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="n">
-        <v>1</v>
-      </c>
-      <c r="G63" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. Townsfolk abilities yield false info. Each day, if no-one is executed, evil wins.</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
       <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>Courtier</t>
+          <t>Yaggababble</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a character: they are drunk for 3 nights &amp; 3 days.</t>
+          <t>You start knowing a secret phrase. For each time you said it publicly today, a player might die.</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
       <c r="G64" t="inlineStr"/>
-      <c r="H64" t="n">
-        <v>1</v>
-      </c>
+      <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>Dreamer</t>
+          <t>Fang Gu</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Each night, choose a player (not yourself or Travellers): you learn 1 good &amp; 1 evil character, 1 of which is correct.</t>
+          <t>Each night*, choose a player: they die. The 1st Outsider this kills becomes an evil Fang Gu &amp; you die instead. [+1 Outsider]</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -1850,7 +1860,7 @@
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>Empath</t>
+          <t>Acrobat</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1860,7 +1870,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Each night, you learn how many of your 2 alive neighbors are evil.</t>
+          <t>Each night*, choose a player: if they are or become drunk or poisoned tonight, you die.</t>
         </is>
       </c>
       <c r="E66" t="n">
@@ -1873,40 +1883,40 @@
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
-          <t>Engineer</t>
+          <t>Zombuul</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose which Minions or which Demon is in play.</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
+          <t>Each night*, if no-one died today, choose a player: they die. The 1st time you die, you live but register as dead.</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>1</v>
+      </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
-      <c r="H67" t="n">
-        <v>1</v>
-      </c>
+      <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>Exorcist</t>
+          <t>Lil' Monsta</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Each night*, choose a player (different to last night): the Demon, if chosen, learns who you are then doesn't wake tonight.</t>
+          <t>Each night, Minions choose who babysits Lil' Monsta &amp; 'is the Demon'. Each night*, a player might die. [+1 Minion]</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -1919,7 +1929,7 @@
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>Farmer</t>
+          <t>Alsaahir</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1929,18 +1939,20 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>When you die at night, an alive good player becomes a Farmer.</t>
+          <t>Each day, if you publicly guess which players are Minion(s) and which are Demon(s), good wins.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
+      <c r="G69" t="n">
+        <v>1</v>
+      </c>
       <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>Fisherman</t>
+          <t>Alchemist</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1950,20 +1962,18 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Once per game, during the day, visit the Storyteller for some advice to help your team win.</t>
+          <t>You have a Minion ability. When using this, the Storyteller may prompt you to choose differently.</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
-      <c r="H70" t="n">
-        <v>1</v>
-      </c>
+      <c r="H70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>Flowergirl</t>
+          <t>Amnesiac</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1973,33 +1983,35 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Each night*, you learn if a Demon voted today.</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>1</v>
-      </c>
+          <t>You do not know what your ability is. Each day, privately guess what it is: you learn how accurate you are.</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
+      <c r="G71" t="n">
+        <v>1</v>
+      </c>
       <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>Fool</t>
+          <t>Lord of Typhon</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>The 1st time you die, you don't.</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr"/>
+          <t>Each night*, choose a player: they die. [Evil characters are in a line. You are in the middle. +1 Minion. -? to +? Outsiders]</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
@@ -2007,17 +2019,17 @@
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>Gambler</t>
+          <t>No Dashii</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Townsfolk</t>
+          <t>Demons</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Each night*, choose a player &amp; guess their character: if you guess wrong, you die.</t>
+          <t>Each night*, choose a player: they die. Your 2 Townsfolk neighbors are poisoned.</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -2030,7 +2042,7 @@
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>Bounty Hunter</t>
+          <t>Artist</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2040,20 +2052,20 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>You start knowing 1 evil player. If the player you know dies, you learn another evil player tonight. [1 Townsfolk is evil]</t>
+          <t>Once per game, during the day, privately ask the Storyteller any yes/no question.</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
-      <c r="F74" t="n">
-        <v>1</v>
-      </c>
+      <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Atheist</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2063,12 +2075,10 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Each night, you learn which alignment the Storyteller believes is winning: good, evil, or neither.</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>1</v>
-      </c>
+          <t>The Storyteller can break the game rules, and if executed, good wins, even if you are dead. [No evil characters]</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
@@ -2076,7 +2086,7 @@
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>Gossip</t>
+          <t>Banshee</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2086,20 +2096,18 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Each day, you may make a public statement. Tonight, if it was true, a player dies.</t>
+          <t>No quoted ability text found</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr"/>
-      <c r="G76" t="n">
-        <v>1</v>
-      </c>
+      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>Grandmother</t>
+          <t>Balloonist</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2109,20 +2117,20 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>You start knowing a good player &amp; their character. If the Demon kills them, you die too.</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night, you learn a player of a different character type than last night. [+0 or +1 Outsider]</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>Huntsman</t>
+          <t>Cannibal</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2132,20 +2140,18 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a living player: the Damsel, if chosen, becomes a not-in-play Townsfolk. [+the Damsel]</t>
+          <t>You have the ability of the recently killed executee. If they are evil, you are poisoned until a good player dies by execution.</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
-      <c r="H78" t="n">
-        <v>1</v>
-      </c>
+      <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>Innkeeper</t>
+          <t>Chambermaid</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2155,7 +2161,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Each night*, choose 2 players: they can't die tonight, but 1 is drunk until dusk.</t>
+          <t>Each night, choose 2 alive players (not yourself): you learn how many woke tonight due to their ability.</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2168,7 +2174,7 @@
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>Investigator</t>
+          <t>Chef</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2178,7 +2184,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>You start knowing that 1 of 2 players is a particular Minion.</t>
+          <t>You start knowing how many pairs of evil players there are.</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -2191,7 +2197,7 @@
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>Juggler</t>
+          <t>Choirboy</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2201,7 +2207,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>On your 1st day, publicly guess up to 5 players' characters. That night, you learn how many you got correct.</t>
+          <t>If the Demon kills the King, you learn which player is the Demon. [+the King]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -2212,7 +2218,7 @@
     <row r="82">
       <c r="B82" t="inlineStr">
         <is>
-          <t>Cult Leader</t>
+          <t>Clockmaker</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2222,20 +2228,20 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Each night, you become the alignment of an alive neighbor. If all good players choose to join your cult, your team wins.</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" t="inlineStr"/>
+          <t>You start knowing how many steps from the Demon to its nearest Minion.</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>King</t>
+          <t>Courtier</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2245,20 +2251,20 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Each night, if the dead equal or outnumber the living, you learn 1 alive character. The Demon knows you are the King.</t>
-        </is>
-      </c>
-      <c r="E83" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night, choose a character: they are drunk for 3 nights &amp; 3 days.</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
+      <c r="H83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>Knight</t>
+          <t>Dreamer</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2268,20 +2274,20 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>You start knowing 2 players that are not the Demon.</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr"/>
-      <c r="F84" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night, choose a player (not yourself or Travellers): you learn 1 good &amp; 1 evil character, 1 of which is correct.</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
         <is>
-          <t>Librarian</t>
+          <t>Empath</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2291,20 +2297,20 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>You start knowing that 1 of 2 players is a particular Outsider. (Or that zero are in play.)</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr"/>
-      <c r="F85" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night, you learn how many of your 2 alive neighbors are evil.</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>Lycanthrope</t>
+          <t>Engineer</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2314,20 +2320,20 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Each night*, choose an alive player. If good, they die &amp; the Demon doesn’t kill tonight. One good player registers as evil.</t>
-        </is>
-      </c>
-      <c r="E86" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night, choose which Minions or which Demon is in play.</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
+      <c r="H86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>Magician</t>
+          <t>Exorcist</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2337,10 +2343,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>The Demon thinks you are a Minion. Minions think you are a Demon.</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr"/>
+          <t>Each night*, choose a player (different to last night): the Demon, if chosen, learns who you are then doesn't wake tonight.</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>1</v>
+      </c>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
@@ -2348,7 +2356,7 @@
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>Mathematician</t>
+          <t>Farmer</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2358,12 +2366,10 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Each night, you learn how many players' abilities worked abnormally (since dawn) due to another character's ability.</t>
-        </is>
-      </c>
-      <c r="E88" t="n">
-        <v>1</v>
-      </c>
+          <t>When you die at night, an alive good player becomes a Farmer.</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
@@ -2371,7 +2377,7 @@
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>Mayor</t>
+          <t>Fisherman</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2381,18 +2387,20 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>If only 3 players live &amp; no execution occurs, your team wins. If you die at night, another player might die instead.</t>
+          <t>Once per game, during the day, visit the Storyteller for some advice to help your team win.</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
+      <c r="H89" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>Fortune Teller</t>
+          <t>Flowergirl</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2402,7 +2410,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Each night, choose 2 players: you learn if either is a Demon. There is a good player that registers as a Demon to you.</t>
+          <t>Each night*, you learn if a Demon voted today.</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -2415,7 +2423,7 @@
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>Minstrel</t>
+          <t>Fool</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2425,7 +2433,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>When a Minion dies by execution, all other players (except Travellers) are drunk until dusk tomorrow.</t>
+          <t>The 1st time you die, you don't.</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -2436,7 +2444,7 @@
     <row r="92">
       <c r="B92" t="inlineStr">
         <is>
-          <t>Monk</t>
+          <t>Gambler</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2446,7 +2454,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Each night*, choose a player (not yourself): they are safe from the Demon tonight.</t>
+          <t>Each night*, choose a player &amp; guess their character: if you guess wrong, you die.</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -2459,7 +2467,7 @@
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>Nightwatchman</t>
+          <t>General</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2469,20 +2477,20 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a player: they learn you are the Nightwatchman.</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr"/>
+          <t>Each night, you learn which alignment the Storyteller believes is winning: good, evil, or neither.</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>1</v>
+      </c>
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
-      <c r="H93" t="n">
-        <v>1</v>
-      </c>
+      <c r="H93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>Oracle</t>
+          <t>Bounty Hunter</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2492,20 +2500,20 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Each night*, you learn how many dead players are evil.</t>
-        </is>
-      </c>
-      <c r="E94" t="n">
-        <v>1</v>
-      </c>
-      <c r="F94" t="inlineStr"/>
+          <t>You start knowing 1 evil player. If the player you know dies, you learn another evil player tonight. [1 Townsfolk is evil]</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="n">
+        <v>1</v>
+      </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>Noble</t>
+          <t>Gossip</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2515,20 +2523,20 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>You start knowing 3 players, 1 and only 1 of which is evil.</t>
+          <t>Each day, you may make a public statement. Tonight, if it was true, a player dies.</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
-      <c r="F95" t="n">
-        <v>1</v>
-      </c>
-      <c r="G95" t="inlineStr"/>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="n">
+        <v>1</v>
+      </c>
       <c r="H95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>High Priestess</t>
+          <t>Grandmother</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2538,20 +2546,20 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Each night, learn which player the Storyteller believes you should talk to most.</t>
-        </is>
-      </c>
-      <c r="E96" t="n">
-        <v>1</v>
-      </c>
-      <c r="F96" t="inlineStr"/>
+          <t>You start knowing a good player &amp; their character. If the Demon kills them, you die too.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="n">
+        <v>1</v>
+      </c>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="B97" t="inlineStr">
         <is>
-          <t>Pacifist</t>
+          <t>Cult Leader</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2561,10 +2569,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Executed good players might not die.</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr"/>
+          <t>Each night, you become the alignment of an alive neighbor. If all good players choose to join your cult, your team wins.</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>1</v>
+      </c>
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
@@ -2572,7 +2582,7 @@
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>Philosopher</t>
+          <t>Huntsman</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2582,7 +2592,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose a good character: gain that ability. If this character is in play, they are drunk.</t>
+          <t>Once per game, at night, choose a living player: the Damsel, if chosen, becomes a not-in-play Townsfolk. [+the Damsel]</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -2595,7 +2605,7 @@
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
-          <t>Pixie</t>
+          <t>Innkeeper</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2605,20 +2615,20 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>You start knowing 1 in-play Townsfolk. If you were mad that you were this character, you gain their ability when they die.</t>
-        </is>
-      </c>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, choose 2 players: they can't die tonight, but 1 is drunk until dusk.</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>Preacher</t>
+          <t>Investigator</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2628,20 +2638,20 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Each night, choose a player: a Minion, if chosen, learns this. All chosen Minions have no ability.</t>
-        </is>
-      </c>
-      <c r="E100" t="n">
-        <v>1</v>
-      </c>
-      <c r="F100" t="inlineStr"/>
+          <t>You start knowing that 1 of 2 players is a particular Minion.</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="n">
+        <v>1</v>
+      </c>
       <c r="G100" t="inlineStr"/>
       <c r="H100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>King</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2651,20 +2661,20 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Once per game, at night*, choose a dead player: if they are a Townsfolk, they are resurrected.</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr"/>
+          <t>Each night, if the dead equal or outnumber the living, you learn 1 alive character. The Demon knows you are the King.</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>1</v>
+      </c>
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
-      <c r="H101" t="n">
-        <v>1</v>
-      </c>
+      <c r="H101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
         <is>
-          <t>Sage</t>
+          <t>Juggler</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2674,7 +2684,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>If the Demon kills you, you learn that it is 1 of 2 players.</t>
+          <t>On your 1st day, publicly guess up to 5 players' characters. That night, you learn how many you got correct.</t>
         </is>
       </c>
       <c r="E102" t="inlineStr"/>
@@ -2685,7 +2695,7 @@
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>Ravenkeeper</t>
+          <t>Librarian</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2695,18 +2705,20 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>If you die at night, you are woken to choose a player: you learn their character.</t>
+          <t>You start knowing that 1 of 2 players is a particular Outsider. (Or that zero are in play.)</t>
         </is>
       </c>
       <c r="E103" t="inlineStr"/>
-      <c r="F103" t="inlineStr"/>
+      <c r="F103" t="n">
+        <v>1</v>
+      </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>Sailor</t>
+          <t>Knight</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2716,20 +2728,20 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Each night, choose an alive player: either you or they are drunk until dusk. You can't die.</t>
-        </is>
-      </c>
-      <c r="E104" t="n">
-        <v>1</v>
-      </c>
-      <c r="F104" t="inlineStr"/>
+          <t>You start knowing 2 players that are not the Demon.</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="n">
+        <v>1</v>
+      </c>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>Savant</t>
+          <t>Lycanthrope</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2739,20 +2751,20 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Each day, you may visit the Storyteller to learn 2 things in private: 1 is true &amp; 1 is false.</t>
-        </is>
-      </c>
-      <c r="E105" t="inlineStr"/>
+          <t>Each night*, choose an alive player. If good, they die &amp; the Demon doesn’t kill tonight. One good player registers as evil.</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>1</v>
+      </c>
       <c r="F105" t="inlineStr"/>
-      <c r="G105" t="n">
-        <v>1</v>
-      </c>
+      <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>Seamstress</t>
+          <t>Magician</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2762,20 +2774,18 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Once per game, at night, choose 2 players (not yourself): you learn if they are the same alignment.</t>
+          <t>The Demon thinks you are a Minion. Minions think you are a Demon.</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
-      <c r="H106" t="n">
-        <v>1</v>
-      </c>
+      <c r="H106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="B107" t="inlineStr">
         <is>
-          <t>Shugenja</t>
+          <t>Mayor</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2785,20 +2795,18 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>You start knowing if your closest evil player is clockwise or anti-clockwise. If equidistant, this info is arbitrary.</t>
+          <t>If only 3 players live &amp; no execution occurs, your team wins. If you die at night, another player might die instead.</t>
         </is>
       </c>
       <c r="E107" t="inlineStr"/>
-      <c r="F107" t="n">
-        <v>1</v>
-      </c>
+      <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="B108" t="inlineStr">
         <is>
-          <t>Slayer</t>
+          <t>Mathematician</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2808,20 +2816,20 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Once per game, during the day, publicly choose a player: if they are the Demon, they die.</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr"/>
+          <t>Each night, you learn how many players' abilities worked abnormally (since dawn) due to another character's ability.</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>1</v>
+      </c>
       <c r="F108" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
-      <c r="H108" t="n">
-        <v>1</v>
-      </c>
+      <c r="H108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>Soldier</t>
+          <t>Minstrel</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2831,7 +2839,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>You are safe from the Demon.</t>
+          <t>When a Minion dies by execution, all other players (except Travellers) are drunk until dusk tomorrow.</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
@@ -2842,7 +2850,7 @@
     <row r="110">
       <c r="B110" t="inlineStr">
         <is>
-          <t>Steward</t>
+          <t>Monk</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2852,20 +2860,20 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>You start knowing 1 good player.</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr"/>
-      <c r="F110" t="n">
-        <v>1</v>
-      </c>
+          <t>Each night*, choose a player (not yourself): they are safe from the Demon tonight.</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="B111" t="inlineStr">
         <is>
-          <t>Undertaker</t>
+          <t>Fortune Teller</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2875,7 +2883,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Each night*, you learn which character died by execution today.</t>
+          <t>Each night, choose 2 players: you learn if either is a Demon. There is a good player that registers as a Demon to you.</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -2888,7 +2896,7 @@
     <row r="112">
       <c r="B112" t="inlineStr">
         <is>
-          <t>Virgin</t>
+          <t>Noble</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2898,18 +2906,20 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>The 1st time you are nominated, if the nominator is a Townsfolk, they are executed immediately.</t>
+          <t>You start knowing 3 players, 1 and only 1 of which is evil.</t>
         </is>
       </c>
       <c r="E112" t="inlineStr"/>
-      <c r="F112" t="inlineStr"/>
+      <c r="F112" t="n">
+        <v>1</v>
+      </c>
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="B113" t="inlineStr">
         <is>
-          <t>Washerwoman</t>
+          <t>Nightwatchman</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2919,30 +2929,30 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>You start knowing that 1 of 2 players is a particular Townsfolk.</t>
+          <t>Once per game, at night, choose a player: they learn you are the Nightwatchman.</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
-      <c r="F113" t="n">
-        <v>1</v>
-      </c>
+      <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
+      <c r="H113" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
       <c r="B114" t="inlineStr">
         <is>
-          <t>Al-Hadikhia</t>
+          <t>Oracle</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Each night*, you may choose 3 players (all players learn who): each silently chooses to live or die, but if all live, all die.</t>
+          <t>Each night*, you learn how many dead players are evil.</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -2955,7 +2965,7 @@
     <row r="115">
       <c r="B115" t="inlineStr">
         <is>
-          <t>Poppy Grower</t>
+          <t>Pacifist</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2965,7 +2975,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Minions &amp; Demons do not know each other. If you die, they learn who each other are that night.</t>
+          <t>Executed good players might not die.</t>
         </is>
       </c>
       <c r="E115" t="inlineStr"/>
@@ -2976,66 +2986,68 @@
     <row r="116">
       <c r="B116" t="inlineStr">
         <is>
-          <t>Kazali</t>
+          <t>Philosopher</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. [You choose which players are which Minions. -? to +? Outsiders]</t>
-        </is>
-      </c>
-      <c r="E116" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night, choose a good character: gain that ability. If this character is in play, they are drunk.</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
-      <c r="H116" t="inlineStr"/>
+      <c r="H116" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117">
       <c r="B117" t="inlineStr">
         <is>
-          <t>Imp</t>
+          <t>Pixie</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. If you kill yourself this way, a Minion becomes the Imp.</t>
-        </is>
-      </c>
-      <c r="E117" t="n">
-        <v>1</v>
-      </c>
-      <c r="F117" t="inlineStr"/>
+          <t>You start knowing 1 in-play Townsfolk. If you were mad that you were this character, you gain their ability when they die.</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="n">
+        <v>1</v>
+      </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="B118" t="inlineStr">
         <is>
-          <t>Leviathan</t>
+          <t>High Priestess</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>If more than 1 good player is executed, evil wins. All players know you are in play. After day 5, evil wins.</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr"/>
+          <t>Each night, learn which player the Storyteller believes you should talk to most.</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>1</v>
+      </c>
       <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
@@ -3043,17 +3055,17 @@
     <row r="119">
       <c r="B119" t="inlineStr">
         <is>
-          <t>Legion</t>
+          <t>Preacher</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Each night*, a player might die. Executions fail if only evil voted. You register as a Minion too. [Most players are Legion]</t>
+          <t>Each night, choose a player: a Minion, if chosen, learns this. All chosen Minions have no ability.</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3066,32 +3078,30 @@
     <row r="120">
       <c r="B120" t="inlineStr">
         <is>
-          <t>Lleech</t>
+          <t>Professor</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. You start by choosing a player: they are poisoned. You die if &amp; only if they are dead.</t>
-        </is>
-      </c>
-      <c r="E120" t="n">
-        <v>1</v>
-      </c>
-      <c r="F120" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night*, choose a dead player: if they are a Townsfolk, they are resurrected.</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr"/>
       <c r="G120" t="inlineStr"/>
-      <c r="H120" t="inlineStr"/>
+      <c r="H120" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="B121" t="inlineStr">
         <is>
-          <t>Snake Charmer</t>
+          <t>Ravenkeeper</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3101,12 +3111,10 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Each night, choose an alive player: a chosen Demon swaps characters &amp; alignments with you &amp; is then poisoned.</t>
-        </is>
-      </c>
-      <c r="E121" t="n">
-        <v>1</v>
-      </c>
+          <t>If you die at night, you are woken to choose a player: you learn their character.</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr"/>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr"/>
@@ -3114,17 +3122,17 @@
     <row r="122">
       <c r="B122" t="inlineStr">
         <is>
-          <t>Ojo</t>
+          <t>Sailor</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Each night*, choose a character: they die. If they are not in play, the Storyteller chooses who dies.</t>
+          <t>Each night, choose an alive player: either you or they are drunk until dusk. You can't die.</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -3137,7 +3145,7 @@
     <row r="123">
       <c r="B123" t="inlineStr">
         <is>
-          <t>Tea Lady</t>
+          <t>Sage</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3147,7 +3155,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>If both your alive neighbors are good, they can't die.</t>
+          <t>If the Demon kills you, you learn that it is 1 of 2 players.</t>
         </is>
       </c>
       <c r="E123" t="inlineStr"/>
@@ -3158,53 +3166,53 @@
     <row r="124">
       <c r="B124" t="inlineStr">
         <is>
-          <t>Po</t>
+          <t>Savant</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Each night*, you may choose a player: they die. If your last choice was no-one, choose 3 players tonight.</t>
-        </is>
-      </c>
-      <c r="E124" t="n">
-        <v>1</v>
-      </c>
+          <t>Each day, you may visit the Storyteller to learn 2 things in private: 1 is true &amp; 1 is false.</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr"/>
+      <c r="G124" t="n">
+        <v>1</v>
+      </c>
       <c r="H124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="B125" t="inlineStr">
         <is>
-          <t>Pukka</t>
+          <t>Seamstress</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Each night, choose a player: they are poisoned. The previously poisoned player dies then becomes healthy.</t>
-        </is>
-      </c>
-      <c r="E125" t="n">
-        <v>1</v>
-      </c>
+          <t>Once per game, at night, choose 2 players (not yourself): you learn if they are the same alignment.</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
-      <c r="H125" t="inlineStr"/>
+      <c r="H125" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="126">
       <c r="B126" t="inlineStr">
         <is>
-          <t>Town Crier</t>
+          <t>Soldier</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3214,12 +3222,10 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Each night*, you learn if a Minion nominated today.</t>
-        </is>
-      </c>
-      <c r="E126" t="n">
-        <v>1</v>
-      </c>
+          <t>You are safe from the Demon.</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="inlineStr"/>
@@ -3227,28 +3233,30 @@
     <row r="127">
       <c r="B127" t="inlineStr">
         <is>
-          <t>Riot</t>
+          <t>Slayer</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>On day 3, Minions become Riot &amp; nominees die but nominate an alive player immediately. This must happen.</t>
+          <t>Once per game, during the day, publicly choose a player: if they are the Demon, they die.</t>
         </is>
       </c>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
       <c r="G127" t="inlineStr"/>
-      <c r="H127" t="inlineStr"/>
+      <c r="H127" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="128">
       <c r="B128" t="inlineStr">
         <is>
-          <t>Village Idiot</t>
+          <t>Shugenja</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3258,53 +3266,53 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Each night, choose a player: you learn their alignment. [+0 to +2 Village Idiots. 1 of the extras is drunk]</t>
-        </is>
-      </c>
-      <c r="E128" t="n">
-        <v>1</v>
-      </c>
-      <c r="F128" t="inlineStr"/>
+          <t>You start knowing if your closest evil player is clockwise or anti-clockwise. If equidistant, this info is arbitrary.</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="n">
+        <v>1</v>
+      </c>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="B129" t="inlineStr">
         <is>
-          <t>Shabaloth</t>
+          <t>Steward</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Each night*, choose 2 players: they die. A dead player you chose last night might be regurgitated.</t>
-        </is>
-      </c>
-      <c r="E129" t="n">
-        <v>1</v>
-      </c>
-      <c r="F129" t="inlineStr"/>
+          <t>You start knowing 1 good player.</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="n">
+        <v>1</v>
+      </c>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="B130" t="inlineStr">
         <is>
-          <t>Vigormortis</t>
+          <t>Undertaker</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. Minions you kill keep their ability &amp; poison 1 Townsfolk neighbor. [-1 Outsider]</t>
+          <t>Each night*, you learn which character died by execution today.</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -3317,88 +3325,82 @@
     <row r="131">
       <c r="B131" t="inlineStr">
         <is>
-          <t>Yaggababble</t>
+          <t>Virgin</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>You start knowing a secret phrase. For each time you said it publicly today, a player might die.</t>
+          <t>The 1st time you are nominated, if the nominator is a Townsfolk, they are executed immediately.</t>
         </is>
       </c>
       <c r="E131" t="inlineStr"/>
-      <c r="F131" t="n">
-        <v>1</v>
-      </c>
+      <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="B132" t="inlineStr">
         <is>
-          <t>Vortox</t>
+          <t>Poppy Grower</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. Townsfolk abilities yield false info. Each day, if no-one is executed, evil wins.</t>
-        </is>
-      </c>
-      <c r="E132" t="n">
-        <v>1</v>
-      </c>
+          <t>Minions &amp; Demons do not know each other. If you die, they learn who each other are that night.</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
-      <c r="G132" t="n">
-        <v>1</v>
-      </c>
+      <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="B133" t="inlineStr">
         <is>
-          <t>Fang Gu</t>
+          <t>Washerwoman</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. The 1st Outsider this kills becomes an evil Fang Gu &amp; you die instead. [+1 Outsider]</t>
-        </is>
-      </c>
-      <c r="E133" t="n">
-        <v>1</v>
-      </c>
-      <c r="F133" t="inlineStr"/>
+          <t>You start knowing that 1 of 2 players is a particular Townsfolk.</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="n">
+        <v>1</v>
+      </c>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="B134" t="inlineStr">
         <is>
-          <t>Lil' Monsta</t>
+          <t>Snake Charmer</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Each night, Minions choose who babysits Lil' Monsta &amp; 'is the Demon'. Each night*, a player might die. [+1 Minion]</t>
+          <t>Each night, choose an alive player: a chosen Demon swaps characters &amp; alignments with you &amp; is then poisoned.</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -3411,17 +3413,17 @@
     <row r="135">
       <c r="B135" t="inlineStr">
         <is>
-          <t>Zombuul</t>
+          <t>Village Idiot</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Each night*, if no-one died today, choose a player: they die. The 1st time you die, you live but register as dead.</t>
+          <t>Each night, choose a player: you learn their alignment. [+0 to +2 Village Idiots. 1 of the extras is drunk]</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -3434,22 +3436,20 @@
     <row r="136">
       <c r="B136" t="inlineStr">
         <is>
-          <t>Lord of Typhon</t>
+          <t>Tea Lady</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. [Evil characters are in a line. You are in the middle. +1 Minion. -? to +? Outsiders]</t>
-        </is>
-      </c>
-      <c r="E136" t="n">
-        <v>1</v>
-      </c>
+          <t>If both your alive neighbors are good, they can't die.</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr"/>
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="inlineStr"/>
@@ -3457,17 +3457,17 @@
     <row r="137">
       <c r="B137" t="inlineStr">
         <is>
-          <t>No Dashii</t>
+          <t>Town Crier</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Demons</t>
+          <t>Townsfolk</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Each night*, choose a player: they die. Your 2 Townsfolk neighbors are poisoned.</t>
+          <t>Each night*, you learn if a Minion nominated today.</t>
         </is>
       </c>
       <c r="E137" t="n">

</xml_diff>